<commit_message>
Prepare template for figure updates, update readme
</commit_message>
<xml_diff>
--- a/working_files/practice_xcs.xlsx
+++ b/working_files/practice_xcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
   <workbookPr backupFile="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="0" windowWidth="25380" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="-80" yWindow="0" windowWidth="25380" windowHeight="16440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="single" sheetId="27" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="99">
   <si>
     <t>FIELDS Template</t>
   </si>
@@ -270,18 +270,6 @@
     <t>Single Conductor with 1 Ground line</t>
   </si>
   <si>
-    <t>HL_E</t>
-  </si>
-  <si>
-    <t>High Load Existing Scenario</t>
-  </si>
-  <si>
-    <t>HL_P</t>
-  </si>
-  <si>
-    <t>High Load Proposed Scenario</t>
-  </si>
-  <si>
     <t>und_E</t>
   </si>
   <si>
@@ -337,6 +325,12 @@
   </si>
   <si>
     <t>raise3</t>
+  </si>
+  <si>
+    <t>Existing Configuration</t>
+  </si>
+  <si>
+    <t>Proposed Configuration</t>
   </si>
 </sst>
 </file>
@@ -674,7 +668,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -693,6 +687,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -874,7 +870,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -882,6 +878,7 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -889,6 +886,7 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="17"/>
@@ -996,7 +994,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1189,11 +1186,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2076452456"/>
-        <c:axId val="2076459416"/>
+        <c:axId val="2125744792"/>
+        <c:axId val="2125737832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2076452456"/>
+        <c:axId val="2125744792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1215,19 +1212,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076459416"/>
+        <c:crossAx val="2125737832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076459416"/>
+        <c:axId val="2125737832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,21 +1246,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076452456"/>
+        <c:crossAx val="2125744792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1539,11 +1533,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2075879704"/>
-        <c:axId val="2075885288"/>
+        <c:axId val="2128117016"/>
+        <c:axId val="2128122600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2075879704"/>
+        <c:axId val="2128117016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1571,12 +1565,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075885288"/>
+        <c:crossAx val="2128122600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2075885288"/>
+        <c:axId val="2128122600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1605,7 +1599,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075879704"/>
+        <c:crossAx val="2128117016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1946,11 +1940,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2076669960"/>
-        <c:axId val="2076675528"/>
+        <c:axId val="2128175256"/>
+        <c:axId val="2128180840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2076669960"/>
+        <c:axId val="2128175256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1978,12 +1972,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076675528"/>
+        <c:crossAx val="2128180840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076675528"/>
+        <c:axId val="2128180840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2012,7 +2006,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076669960"/>
+        <c:crossAx val="2128175256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2401,11 +2395,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2028326008"/>
-        <c:axId val="2028331592"/>
+        <c:axId val="2081985560"/>
+        <c:axId val="2081991176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2028326008"/>
+        <c:axId val="2081985560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2433,12 +2427,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2028331592"/>
+        <c:crossAx val="2081991176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2028331592"/>
+        <c:axId val="2081991176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2467,7 +2461,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2028326008"/>
+        <c:crossAx val="2081985560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2724,11 +2718,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2075949064"/>
-        <c:axId val="2075954648"/>
+        <c:axId val="2128237112"/>
+        <c:axId val="2128242696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2075949064"/>
+        <c:axId val="2128237112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2756,12 +2750,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075954648"/>
+        <c:crossAx val="2128242696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2075954648"/>
+        <c:axId val="2128242696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2790,7 +2784,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075949064"/>
+        <c:crossAx val="2128237112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3047,11 +3041,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2076750328"/>
-        <c:axId val="2076755912"/>
+        <c:axId val="2128295608"/>
+        <c:axId val="2128301192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2076750328"/>
+        <c:axId val="2128295608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3079,12 +3073,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076755912"/>
+        <c:crossAx val="2128301192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076755912"/>
+        <c:axId val="2128301192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3113,7 +3107,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076750328"/>
+        <c:crossAx val="2128295608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3370,11 +3364,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2076006680"/>
-        <c:axId val="2076012264"/>
+        <c:axId val="2128353944"/>
+        <c:axId val="2128359528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2076006680"/>
+        <c:axId val="2128353944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3402,12 +3396,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076012264"/>
+        <c:crossAx val="2128359528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076012264"/>
+        <c:axId val="2128359528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3436,7 +3430,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076006680"/>
+        <c:crossAx val="2128353944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3483,7 +3477,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3694,11 +3687,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2076791960"/>
-        <c:axId val="2076797544"/>
+        <c:axId val="2128411624"/>
+        <c:axId val="2128417208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2076791960"/>
+        <c:axId val="2128411624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3720,19 +3713,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076797544"/>
+        <c:crossAx val="2128417208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076797544"/>
+        <c:axId val="2128417208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3755,21 +3747,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076791960"/>
+        <c:crossAx val="2128411624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4009,11 +3999,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2075627992"/>
-        <c:axId val="2075633576"/>
+        <c:axId val="2124516024"/>
+        <c:axId val="2124510440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2075627992"/>
+        <c:axId val="2124516024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4042,12 +4032,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075633576"/>
+        <c:crossAx val="2124510440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2075633576"/>
+        <c:axId val="2124510440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4077,7 +4067,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075627992"/>
+        <c:crossAx val="2124516024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4120,7 +4110,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>HL_E</c:v>
+              <c:v>Existing Configuration</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -4384,11 +4374,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2075686104"/>
-        <c:axId val="2075691688"/>
+        <c:axId val="2124460344"/>
+        <c:axId val="2124454760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2075686104"/>
+        <c:axId val="2124460344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4417,12 +4407,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075691688"/>
+        <c:crossAx val="2124454760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2075691688"/>
+        <c:axId val="2124454760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4452,7 +4442,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075686104"/>
+        <c:crossAx val="2124460344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4495,11 +4485,12 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>HL_P</c:v>
+              <c:v>Proposed Configuration</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4758,11 +4749,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2075743096"/>
-        <c:axId val="2075748680"/>
+        <c:axId val="2126972136"/>
+        <c:axId val="2126977720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2075743096"/>
+        <c:axId val="2126972136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4784,18 +4775,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075748680"/>
+        <c:crossAx val="2126977720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2075748680"/>
+        <c:axId val="2126977720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4818,19 +4810,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075743096"/>
+        <c:crossAx val="2126972136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5129,11 +5123,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2076493512"/>
-        <c:axId val="2076499096"/>
+        <c:axId val="2125648744"/>
+        <c:axId val="2125643160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2076493512"/>
+        <c:axId val="2125648744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5161,12 +5155,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076499096"/>
+        <c:crossAx val="2125643160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076499096"/>
+        <c:axId val="2125643160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5195,7 +5189,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076493512"/>
+        <c:crossAx val="2125648744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5494,11 +5488,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2076508808"/>
-        <c:axId val="2076514456"/>
+        <c:axId val="2125589464"/>
+        <c:axId val="2125583880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2076508808"/>
+        <c:axId val="2125589464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5526,12 +5520,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076514456"/>
+        <c:crossAx val="2125583880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076514456"/>
+        <c:axId val="2125583880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5560,7 +5554,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076508808"/>
+        <c:crossAx val="2125589464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5859,11 +5853,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2076590152"/>
-        <c:axId val="2076595736"/>
+        <c:axId val="2125530936"/>
+        <c:axId val="2125525352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2076590152"/>
+        <c:axId val="2125530936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5891,12 +5885,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076595736"/>
+        <c:crossAx val="2125525352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076595736"/>
+        <c:axId val="2125525352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5925,7 +5919,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076590152"/>
+        <c:crossAx val="2125530936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6224,11 +6218,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2075819720"/>
-        <c:axId val="2075825304"/>
+        <c:axId val="2125472392"/>
+        <c:axId val="2125466808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2075819720"/>
+        <c:axId val="2125472392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6256,12 +6250,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075825304"/>
+        <c:crossAx val="2125466808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2075825304"/>
+        <c:axId val="2125466808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6290,7 +6284,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075819720"/>
+        <c:crossAx val="2125472392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6577,11 +6571,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2076647832"/>
-        <c:axId val="2076653416"/>
+        <c:axId val="2128057048"/>
+        <c:axId val="2128062632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2076647832"/>
+        <c:axId val="2128057048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6609,12 +6603,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076653416"/>
+        <c:crossAx val="2128062632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076653416"/>
+        <c:axId val="2128062632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6643,7 +6637,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076647832"/>
+        <c:crossAx val="2128057048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8086,7 +8080,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C5" s="53" t="s">
         <v>37</v>
@@ -8195,7 +8189,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C7" s="54" t="s">
         <v>35</v>
@@ -8655,7 +8649,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C5" s="76" t="s">
         <v>26</v>
@@ -8764,7 +8758,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C7" s="77" t="s">
         <v>24</v>
@@ -9396,7 +9390,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C5" s="61" t="s">
         <v>26</v>
@@ -9505,7 +9499,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C7" s="62" t="s">
         <v>24</v>
@@ -10316,7 +10310,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C5" s="76" t="s">
         <v>24</v>
@@ -10795,7 +10789,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="82" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C5" s="76" t="s">
         <v>24</v>
@@ -11274,7 +11268,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="82" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C5" s="76" t="s">
         <v>24</v>
@@ -12092,7 +12086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -12526,8 +12520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -12666,7 +12660,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>24</v>
@@ -12775,7 +12769,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>26</v>
@@ -13172,7 +13166,7 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -13311,7 +13305,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>24</v>
@@ -13420,7 +13414,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>26</v>
@@ -13956,7 +13950,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>35</v>
@@ -14065,7 +14059,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>38</v>
@@ -14601,7 +14595,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>35</v>
@@ -14710,7 +14704,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>38</v>
@@ -15235,7 +15229,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C5" s="76" t="s">
         <v>39</v>
@@ -15346,7 +15340,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C7" s="77" t="s">
         <v>41</v>
@@ -15876,7 +15870,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C5" s="76" t="s">
         <v>35</v>
@@ -15991,7 +15985,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C7" s="77" t="s">
         <v>38</v>
@@ -16527,7 +16521,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C5" s="46" t="s">
         <v>37</v>
@@ -16636,7 +16630,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C7" s="47" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Update figures, add gouraud shading to pcolormesh plot
</commit_message>
<xml_diff>
--- a/working_files/practice_xcs.xlsx
+++ b/working_files/practice_xcs.xlsx
@@ -947,7 +947,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1125,11 +1124,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95013888"/>
-        <c:axId val="95024256"/>
+        <c:axId val="147516416"/>
+        <c:axId val="147400192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95013888"/>
+        <c:axId val="147516416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1150,16 +1149,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95024256"/>
+        <c:crossAx val="147400192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95024256"/>
+        <c:axId val="147400192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1181,25 +1179,23 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95013888"/>
+        <c:crossAx val="147516416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1221,7 +1217,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1447,11 +1442,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="96171520"/>
-        <c:axId val="96173440"/>
+        <c:axId val="155105536"/>
+        <c:axId val="155115904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96171520"/>
+        <c:axId val="155105536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1472,16 +1467,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96173440"/>
+        <c:crossAx val="155115904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96173440"/>
+        <c:axId val="155115904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1503,25 +1497,23 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96171520"/>
+        <c:crossAx val="155105536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1762,11 +1754,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="100924800"/>
-        <c:axId val="100934784"/>
+        <c:axId val="155712512"/>
+        <c:axId val="155731072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100924800"/>
+        <c:axId val="155712512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1790,12 +1782,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100934784"/>
+        <c:crossAx val="155731072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100934784"/>
+        <c:axId val="155731072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1820,7 +1812,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100924800"/>
+        <c:crossAx val="155712512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1833,7 +1825,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2134,11 +2126,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="100969472"/>
-        <c:axId val="100979840"/>
+        <c:axId val="155803648"/>
+        <c:axId val="155805568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100969472"/>
+        <c:axId val="155803648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2162,12 +2154,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100979840"/>
+        <c:crossAx val="155805568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100979840"/>
+        <c:axId val="155805568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2192,7 +2184,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100969472"/>
+        <c:crossAx val="155803648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2205,7 +2197,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2554,11 +2546,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="101016320"/>
-        <c:axId val="101018240"/>
+        <c:axId val="155845376"/>
+        <c:axId val="155847296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101016320"/>
+        <c:axId val="155845376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2582,12 +2574,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101018240"/>
+        <c:crossAx val="155847296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101018240"/>
+        <c:axId val="155847296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2612,7 +2604,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101016320"/>
+        <c:crossAx val="155845376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2625,7 +2617,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2842,11 +2834,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="3044864"/>
-        <c:axId val="3046784"/>
+        <c:axId val="155870720"/>
+        <c:axId val="155872640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="3044864"/>
+        <c:axId val="155870720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2870,12 +2862,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3046784"/>
+        <c:crossAx val="155872640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="3046784"/>
+        <c:axId val="155872640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2900,7 +2892,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3044864"/>
+        <c:crossAx val="155870720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2913,7 +2905,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3130,11 +3122,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="65509632"/>
-        <c:axId val="65524096"/>
+        <c:axId val="156424448"/>
+        <c:axId val="156238208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65509632"/>
+        <c:axId val="156424448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3158,12 +3150,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65524096"/>
+        <c:crossAx val="156238208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65524096"/>
+        <c:axId val="156238208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3188,7 +3180,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65509632"/>
+        <c:crossAx val="156424448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3201,7 +3193,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3418,11 +3410,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="124999936"/>
-        <c:axId val="125018496"/>
+        <c:axId val="156302336"/>
+        <c:axId val="155391104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124999936"/>
+        <c:axId val="156302336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3446,12 +3438,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125018496"/>
+        <c:crossAx val="155391104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125018496"/>
+        <c:axId val="155391104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3476,7 +3468,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124999936"/>
+        <c:crossAx val="156302336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3489,7 +3481,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3706,11 +3698,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="125074432"/>
-        <c:axId val="125080704"/>
+        <c:axId val="156615040"/>
+        <c:axId val="156616960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125074432"/>
+        <c:axId val="156615040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3734,12 +3726,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125080704"/>
+        <c:crossAx val="156616960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125080704"/>
+        <c:axId val="156616960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3764,7 +3756,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125074432"/>
+        <c:crossAx val="156615040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3777,7 +3769,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3982,11 +3974,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95080448"/>
-        <c:axId val="95082368"/>
+        <c:axId val="148178048"/>
+        <c:axId val="148179968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95080448"/>
+        <c:axId val="148178048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4010,12 +4002,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95082368"/>
+        <c:crossAx val="148179968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95082368"/>
+        <c:axId val="148179968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4040,7 +4032,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95080448"/>
+        <c:crossAx val="148178048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4053,7 +4045,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4318,11 +4310,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95167232"/>
-        <c:axId val="95169152"/>
+        <c:axId val="153707648"/>
+        <c:axId val="153709568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95167232"/>
+        <c:axId val="153707648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4346,12 +4338,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95169152"/>
+        <c:crossAx val="153709568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95169152"/>
+        <c:axId val="153709568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4376,7 +4368,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95167232"/>
+        <c:crossAx val="153707648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4389,7 +4381,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4654,11 +4646,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95217152"/>
-        <c:axId val="95219072"/>
+        <c:axId val="153785856"/>
+        <c:axId val="153787776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95217152"/>
+        <c:axId val="153785856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4682,12 +4674,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95219072"/>
+        <c:crossAx val="153787776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95219072"/>
+        <c:axId val="153787776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4712,7 +4704,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95217152"/>
+        <c:crossAx val="153785856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4725,7 +4717,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4990,11 +4982,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95578368"/>
-        <c:axId val="95592832"/>
+        <c:axId val="154921216"/>
+        <c:axId val="153616768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95578368"/>
+        <c:axId val="154921216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5018,12 +5010,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95592832"/>
+        <c:crossAx val="153616768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95592832"/>
+        <c:axId val="153616768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5048,7 +5040,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95578368"/>
+        <c:crossAx val="154921216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5061,7 +5053,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5083,7 +5075,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -5321,11 +5312,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95665152"/>
-        <c:axId val="95671424"/>
+        <c:axId val="153672704"/>
+        <c:axId val="153678976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95665152"/>
+        <c:axId val="153672704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5346,16 +5337,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95671424"/>
+        <c:crossAx val="153678976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95671424"/>
+        <c:axId val="153678976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5377,25 +5367,23 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95665152"/>
+        <c:crossAx val="153672704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5550,7 +5538,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>57.928500000000007</c:v>
+                  <c:v>-5.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -5598,7 +5586,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>57.928500000000007</c:v>
+                  <c:v>-5.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -5607,11 +5595,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="140534144"/>
-        <c:axId val="140536064"/>
+        <c:axId val="155468544"/>
+        <c:axId val="155470464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="140534144"/>
+        <c:axId val="155468544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5636,12 +5624,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140536064"/>
+        <c:crossAx val="155470464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="140536064"/>
+        <c:axId val="155470464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5667,7 +5655,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140534144"/>
+        <c:crossAx val="155468544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5681,7 +5669,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000366" l="0.70000000000000262" r="0.70000000000000262" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000262" r="0.70000000000000262" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5940,11 +5928,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95813632"/>
-        <c:axId val="95815552"/>
+        <c:axId val="155546368"/>
+        <c:axId val="155548288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95813632"/>
+        <c:axId val="155546368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5968,12 +5956,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95815552"/>
+        <c:crossAx val="155548288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95815552"/>
+        <c:axId val="155548288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5998,7 +5986,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95813632"/>
+        <c:crossAx val="155546368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6011,7 +5999,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6270,11 +6258,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="96117504"/>
-        <c:axId val="96119424"/>
+        <c:axId val="155633152"/>
+        <c:axId val="155635072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96117504"/>
+        <c:axId val="155633152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6298,12 +6286,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96119424"/>
+        <c:crossAx val="155635072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96119424"/>
+        <c:axId val="155635072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6328,7 +6316,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96117504"/>
+        <c:crossAx val="155633152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6341,7 +6329,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.7000000000000024" r="0.7000000000000024" t="0.75000000000000344" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000251" r="0.70000000000000251" t="0.75000000000000355" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -15317,7 +15305,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -15708,10 +15696,10 @@
       <c r="H20" s="34"/>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
       <c r="N20" s="65"/>
     </row>
     <row r="21" spans="3:14">
+      <c r="K21" s="80"/>
       <c r="N21" s="65"/>
     </row>
     <row r="22" spans="3:14">

</xml_diff>